<commit_message>
Update patch version + SLPS
</commit_message>
<xml_diff>
--- a/patch/SLPS/scripts/dfFinal.xlsx
+++ b/patch/SLPS/scripts/dfFinal.xlsx
@@ -8503,14 +8503,14 @@
         <is>
           <t xml:space="preserve">//Text $14D58
 #WRITE(ptr,$5894)
-Even Thought They're Rebels[END]
+Even Though They're Rebels[END]
 </t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Even Thought They're Rebels[END]
+Even Though They're Rebels[END]
 </t>
         </is>
       </c>
@@ -9433,14 +9433,14 @@
         <is>
           <t xml:space="preserve">//Text $14AC8
 #WRITE(ptr,$5910)
-What Does the Letter Mean?[END]
+Our Intent?[END]
 </t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
         <is>
           <t xml:space="preserve">
-What Does the Letter Mean?[END]
+Our Intent?[END]
 </t>
         </is>
       </c>
@@ -9553,14 +9553,14 @@
         <is>
           <t xml:space="preserve">//Text $14A58
 #WRITE(ptr,$5920)
-Heidelberg is North Through the Forest[END]
+Heidelberg is North through the Forest[END]
 </t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Heidelberg is North Through the Forest[END]
+Heidelberg is North through the Forest[END]
 </t>
         </is>
       </c>
@@ -9583,14 +9583,14 @@
         <is>
           <t xml:space="preserve">//Text $14A48
 #WRITE(ptr,$5924)
-Let's leave the Forest Through the North[END]
+Let's Leave the Forest through the North[END]
 </t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Let's leave the Forest Through the North[END]
+Let's Leave the Forest through the North[END]
 </t>
         </is>
       </c>
@@ -10033,14 +10033,14 @@
         <is>
           <t xml:space="preserve">//Text $148D8
 #WRITE(ptr,$5960)
-Why was this place Abandoned?[END]
+Why was this Place Abandoned?[END]
 </t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Why was this place Abandoned?[END]
+Why was this Place Abandoned?[END]
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
SLPS + Skit Titles
</commit_message>
<xml_diff>
--- a/patch/SLPS/scripts/dfFinal.xlsx
+++ b/patch/SLPS/scripts/dfFinal.xlsx
@@ -5443,14 +5443,14 @@
         <is>
           <t xml:space="preserve">//Text $15640
 #WRITE(ptr,$56FC)
-Monsters in Town?![END]
+Monsters in Town!?[END]
 </t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Monsters in Town?![END]
+Monsters in Town!?[END]
 </t>
         </is>
       </c>
@@ -7813,14 +7813,14 @@
         <is>
           <t xml:space="preserve">//Text $14F58
 #WRITE(ptr,$5838)
-Civil War Outbreak?![END]
+Civil War Outbreak!?[END]
 </t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Civil War Outbreak?![END]
+Civil War Outbreak!?[END]
 </t>
         </is>
       </c>
@@ -15253,14 +15253,14 @@
         <is>
           <t xml:space="preserve">//Text $13888
 #WRITE(ptr,$5C18)
-I'm a Little Rusty[END]
+I'm a Bit Nervous[END]
 </t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
         <is>
           <t xml:space="preserve">
-I'm a Little Rusty[END]
+I'm a Bit Nervous[END]
 </t>
         </is>
       </c>
@@ -15343,14 +15343,14 @@
         <is>
           <t xml:space="preserve">//Text $13840
 #WRITE(ptr,$5C24)
-You're the Future Champion?![END]
+You're the Future Champion!?[END]
 </t>
         </is>
       </c>
       <c r="C498" t="inlineStr">
         <is>
           <t xml:space="preserve">
-You're the Future Champion?![END]
+You're the Future Champion!?[END]
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
New SLPS + Skit Titles + Ver. # Update
</commit_message>
<xml_diff>
--- a/patch/SLPS/scripts/dfFinal.xlsx
+++ b/patch/SLPS/scripts/dfFinal.xlsx
@@ -9013,14 +9013,14 @@
         <is>
           <t xml:space="preserve">//Text $14C00
 #WRITE(ptr,$58D8)
-Neuestadt is Northwest of Lienea[END]
+Neuestadt is Southeast of Lienea[END]
 </t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Neuestadt is Northwest of Lienea[END]
+Neuestadt is Southeast of Lienea[END]
 </t>
         </is>
       </c>
@@ -9043,14 +9043,14 @@
         <is>
           <t xml:space="preserve">//Text $14BE0
 #WRITE(ptr,$58DC)
-Lienea is Southeast of Neuestadt[END]
+Southeast from Lienea is Neuestadt[END]
 </t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Lienea is Southeast of Neuestadt[END]
+Southeast from Lienea is Neuestadt[END]
 </t>
         </is>
       </c>

</xml_diff>